<commit_message>
close #192: Fix duplicate description/values ​​relationship errors
</commit_message>
<xml_diff>
--- a/input_data/data_errors_11/valores.xlsx
+++ b/input_data/data_errors_11/valores.xlsx
@@ -31,19 +31,19 @@
     <t xml:space="preserve">2-2030-O</t>
   </si>
   <si>
-    <t xml:space="preserve">2-2050-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-2030-P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-2050-P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-2015</t>
+    <t xml:space="preserve">2-2090-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML-2030-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">777-2080-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88-2015</t>
   </si>
   <si>
     <t xml:space="preserve">5-2015</t>
@@ -461,7 +461,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>